<commit_message>
john-testing-rdc for sys2 done
</commit_message>
<xml_diff>
--- a/summation_of_time.xlsx
+++ b/summation_of_time.xlsx
@@ -442,432 +442,432 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>47.9</v>
+        <v>479</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>31.3</v>
+        <v>745</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>30.8</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>58.4</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>109.2</v>
+        <v>2610</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>35.8</v>
+        <v>2859</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>72.8</v>
+        <v>3552</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>66.90000000000001</v>
+        <v>4149</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>18.3</v>
+        <v>4266</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>18.8</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>13.5</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>128.7</v>
+        <v>5827</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>59.7</v>
+        <v>6296</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>123.3</v>
+        <v>7470</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>81.59999999999999</v>
+        <v>8163</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>198.9</v>
+        <v>10071</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>33.3</v>
+        <v>10206</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>31</v>
+        <v>10483</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>62.7</v>
+        <v>11079</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>81.90000000000001</v>
+        <v>11836</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>51.8</v>
+        <v>12273</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>228.1</v>
+        <v>14503</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>66.5</v>
+        <v>14940</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>40.6</v>
+        <v>15280</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>44.5</v>
+        <v>15685</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>57.9</v>
+        <v>16220</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>33.4</v>
+        <v>16497</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>39.6</v>
+        <v>16860</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>56.1</v>
+        <v>17382</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>66.90000000000001</v>
+        <v>17995</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>34.3</v>
+        <v>18272</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>133.4</v>
+        <v>19572</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>95.40000000000001</v>
+        <v>20393</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>30.8</v>
+        <v>20606</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>165</v>
+        <v>22226</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>176.6</v>
+        <v>23827</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>47.4</v>
+        <v>24125</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>92.09999999999999</v>
+        <v>24999</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>71</v>
+        <v>25617</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>271.1</v>
+        <v>28257</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>27.6</v>
+        <v>28262</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>17.6</v>
+        <v>28411</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>105.1</v>
+        <v>29445</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>254.6</v>
+        <v>31886</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>71.40000000000001</v>
+        <v>32346</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>63.6</v>
+        <v>32911</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>118.2</v>
+        <v>34030</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>55.5</v>
+        <v>34467</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>98.2</v>
+        <v>35394</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>456</v>
+        <v>39856</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>117</v>
+        <v>40570</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>29.8</v>
+        <v>40751</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>151.4</v>
+        <v>42236</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>90.8</v>
+        <v>42993</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>324.4</v>
+        <v>46147</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>243.9</v>
+        <v>48262</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>112.7</v>
+        <v>49146</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>214.9</v>
+        <v>51183</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>169.5</v>
+        <v>52664</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>72.8</v>
+        <v>53223</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>56.2</v>
+        <v>53713</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>64.90000000000001</v>
+        <v>54306</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>183.3</v>
+        <v>56075</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>26.8</v>
+        <v>56160</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>286.2</v>
+        <v>58996</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>49.9</v>
+        <v>59209</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>191.5</v>
+        <v>61075</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>68.09999999999999</v>
+        <v>61565</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>155.5</v>
+        <v>63052</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>447.7</v>
+        <v>67374</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>186.5</v>
+        <v>68792</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>120.9</v>
+        <v>69815</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>561</v>
+        <v>75305</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>208.1</v>
+        <v>76825</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>348.9</v>
+        <v>80106</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>306.4</v>
+        <v>82822</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>248.1</v>
+        <v>84997</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>375.3</v>
+        <v>88502</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>110</v>
+        <v>89227</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>207.3</v>
+        <v>91190</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>418.6</v>
+        <v>95169</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>150.8</v>
+        <v>96259</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>39.5</v>
+        <v>96504</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>123.3</v>
+        <v>97698</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>111.7</v>
+        <v>98692</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>401.3</v>
+        <v>102594</v>
       </c>
     </row>
   </sheetData>

</xml_diff>